<commit_message>
CF paper and slides
</commit_message>
<xml_diff>
--- a/Seminar List.xlsx
+++ b/Seminar List.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\新建文件夹\SANDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenfei/Downloads/Seminar/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" tabRatio="500"/>
+    <workbookView xWindow="300" yWindow="7080" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -81,14 +81,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">TaoStore: Overcoming Asynchronicity in Oblivious Data Storage </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>TaoStore: Overcoming Asynchronicity in Oblivious Data Storage slides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>2016/6/29
 15:00-18:00</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -159,14 +151,22 @@
   </si>
   <si>
     <t>CrowdTarget Slides.ppt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>towards practical obivious ram.pdf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PracticalORam.pptx</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,9 +312,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="标题 1" xfId="1" builtinId="16"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -594,25 +594,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="18.625" customWidth="1"/>
+    <col min="1" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="62.5" customWidth="1"/>
-    <col min="6" max="6" width="71.375" customWidth="1"/>
+    <col min="6" max="6" width="71.33203125" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1">
+    <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -627,12 +627,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -641,13 +641,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="12"/>
       <c r="C3" s="6">
@@ -657,13 +657,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1">
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="13"/>
       <c r="C4" s="7">
@@ -673,18 +673,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -693,32 +693,32 @@
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
       <c r="B6" s="17"/>
       <c r="C6" s="3">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" thickBot="1">
+    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="18"/>
       <c r="C7" s="4">
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>

</xml_diff>

<commit_message>
CF Usenix Security 2015
:hand:
</commit_message>
<xml_diff>
--- a/Seminar List.xlsx
+++ b/Seminar List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="300" yWindow="7080" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,27 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>姓名</t>
     <rPh sb="0" eb="1">
       <t>xing'm</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>论文</t>
     <rPh sb="0" eb="1">
       <t>lun'w</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>演讲ppt</t>
     <rPh sb="0" eb="1">
       <t>yan'jiang'g</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>演讲顺序</t>
@@ -54,14 +54,14 @@
     <rPh sb="2" eb="3">
       <t>shun'xu</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>陈飞</t>
     <rPh sb="0" eb="1">
       <t>chen'fei</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>李旭嵘</t>
@@ -74,16 +74,16 @@
     <rPh sb="1" eb="2">
       <t>xiang</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>林昶廷</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2016/6/29
 15:00-18:00</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>讨论时间</t>
@@ -93,7 +93,7 @@
     <rPh sb="2" eb="3">
       <t>shi'jian</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>讨论地点</t>
@@ -103,30 +103,30 @@
     <rPh sb="2" eb="3">
       <t>di'dian</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>曹主201</t>
     <rPh sb="1" eb="2">
       <t>zhu'yao</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Practical Issues with TLS Client Certificate Authentication </t>
   </si>
   <si>
     <t>Practical Issues with TLS Client Certificate Authentication slides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2016/7/6
 15:00-18:00</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>王剑宇</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>邢骏驰</t>
@@ -136,37 +136,83 @@
     <rPh sb="1" eb="2">
       <t>jun'chi</t>
     </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>DevoFlow: Scaling Flow Management for High-Performance Networks∗</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>DevoFlow: Scaling Flow Management for High-Performance Networks slides</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">CrowdTarget: Target-based Detection of Crowdturfing in Online Social Networks (CCS’15) </t>
   </si>
   <si>
     <t>CrowdTarget Slides.ppt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>towards practical obivious ram.pdf</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PracticalORam.pptx</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016/7/1
+13:30-18:00</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>曹主201
+观看usenix security 2015 视频</t>
+    <rPh sb="1" eb="2">
+      <t>zhu'yao</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>guan'k</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>shi'p</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>林昶廷</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>李旭嵘</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>王剑宇</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>朱凯</t>
+    <rPh sb="0" eb="1">
+      <t>zhu'kai</t>
+    </rPh>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,14 +239,14 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="DengXian"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,7 +255,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -249,14 +301,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -268,32 +321,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -310,11 +342,54 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="40%-个性色3" xfId="3" builtinId="39"/>
     <cellStyle name="标题 1" xfId="1" builtinId="16"/>
-    <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="个性色2" xfId="2" builtinId="33"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -592,17 +667,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="83.83203125" customWidth="1"/>
     <col min="6" max="6" width="71.33203125" customWidth="1"/>
     <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
@@ -628,109 +703,199 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="6">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>11</v>
+      <c r="A5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="5">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="3">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="4">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="4">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>